<commit_message>
Modified Assumptions and notes.docx Finished Test_Plan.xls Added defects to Defect Log.xlsx Added review results to SW_C_Code_Review_Template.xls
</commit_message>
<xml_diff>
--- a/docs/V-Cycle Process/Defect Log.xlsx
+++ b/docs/V-Cycle Process/Defect Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele\Documents\Personal\Continental Automotive Program\Cursos\V-Cycle Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele\Documents\Personal\Continental Automotive Program\Practicas\Window Lifter WS Github3\trunk\docs\V-Cycle Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -250,10 +250,22 @@
     <t>Incorrect system clock configuration</t>
   </si>
   <si>
-    <t>magic numbers for led counting</t>
-  </si>
-  <si>
     <t>Direct manipulation of registers</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t>Missing proper function comments</t>
+  </si>
+  <si>
+    <t>Magic numbers for led counting</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Outdated headers didn't list changes done to code</t>
   </si>
 </sst>
 </file>
@@ -787,7 +799,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -798,6 +810,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1148,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L32"/>
+  <dimension ref="B3:L34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,10 +1179,10 @@
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" style="7" customWidth="1"/>
     <col min="10" max="10" width="8.140625" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="28" customWidth="1"/>
@@ -1199,30 +1218,48 @@
       <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="5">
+        <v>42181</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5">
+        <v>42181</v>
+      </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>33</v>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>28</v>
@@ -1232,53 +1269,87 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42184</v>
+      </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="I6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
+        <v>42184</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5">
+        <v>42184</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
@@ -1289,12 +1360,12 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="6"/>
       <c r="K9" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
@@ -1305,12 +1376,12 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="6"/>
       <c r="K10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
@@ -1321,15 +1392,15 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="6"/>
       <c r="K11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1337,15 +1408,15 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="6"/>
       <c r="K12" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1353,15 +1424,15 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="6"/>
       <c r="K13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1369,15 +1440,15 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="6"/>
       <c r="K14" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1385,15 +1456,15 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="6"/>
       <c r="K15" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1401,9 +1472,15 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="6"/>
+      <c r="K16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1411,9 +1488,15 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="6"/>
+      <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1421,9 +1504,9 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1431,9 +1514,9 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1441,9 +1524,9 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1451,9 +1534,9 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1461,9 +1544,9 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1471,9 +1554,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1481,9 +1564,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1491,9 +1574,9 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1501,9 +1584,9 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1511,9 +1594,9 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1521,9 +1604,9 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1531,9 +1614,9 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1541,9 +1624,9 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1551,9 +1634,9 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1561,7 +1644,27 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1574,7 +1677,7 @@
   <dimension ref="B4:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adjusted waitms function in MPC5606B_Wait.c because it was counting faster than expected. Updated Defect Log.xlsx with said issue.
</commit_message>
<xml_diff>
--- a/docs/V-Cycle Process/Defect Log.xlsx
+++ b/docs/V-Cycle Process/Defect Log.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Fail to know why the code compiles even without proper includes.</t>
+  </si>
+  <si>
+    <t>waitms() function isn't working properly. Counts faster than expected.</t>
   </si>
 </sst>
 </file>
@@ -1199,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,8 +1215,8 @@
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54" style="7" customWidth="1"/>
     <col min="10" max="10" width="8.140625" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="28" customWidth="1"/>
@@ -1252,7 +1255,9 @@
       <c r="C4" s="5">
         <v>42181</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1269,14 +1274,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="5">
         <v>42181</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1306,7 +1313,9 @@
       <c r="C6" s="5">
         <v>42184</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1330,7 +1339,9 @@
       <c r="C7" s="5">
         <v>42184</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1360,7 +1371,9 @@
       <c r="C8" s="5">
         <v>42184</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1383,14 +1396,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="5">
         <v>42185</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1420,7 +1435,9 @@
       <c r="C10" s="5">
         <v>42185</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
       <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
@@ -1444,14 +1461,30 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="6"/>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42187</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>